<commit_message>
Update tested gunung harta
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Ptgununghartatransportsolutions/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Ptgununghartatransportsolutions/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Malindoairways\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Ptgununghartatransportsolutions\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B2D06E-E37E-41A2-82FD-24BFA53C5186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F728A578-F095-4E69-943B-1B078F0C3025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="336" yWindow="336" windowWidth="19308" windowHeight="8640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -233,18 +233,9 @@
     <t>GCaptcha_RuleId</t>
   </si>
   <si>
-    <t>RPA021_MOLPAY_Captcha_SiteKey</t>
-  </si>
-  <si>
     <t>RPA_Moon_Cred_Gmail</t>
   </si>
   <si>
-    <t>ReportPage</t>
-  </si>
-  <si>
-    <t>https://b2b.malindoair.com/MalindoAirAgentsPortal/Agents/Statements.aspx</t>
-  </si>
-  <si>
     <t>CaptchaProcess</t>
   </si>
   <si>
@@ -258,6 +249,9 @@
   </si>
   <si>
     <t>Traveloka_CaptchaHandler</t>
+  </si>
+  <si>
+    <t>RPA205_GunungHarta_Captcha_SiteKey</t>
   </si>
 </sst>
 </file>
@@ -634,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -725,7 +719,7 @@
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
@@ -733,24 +727,17 @@
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
       <c r="A8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1">
-      <c r="A9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" t="s">
-        <v>74</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:26" ht="14.3" customHeight="1">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-    </row>
+    <row r="10" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.3" customHeight="1"/>
@@ -1736,7 +1723,6 @@
     <row r="993" ht="14.3" customHeight="1"/>
     <row r="994" ht="14.3" customHeight="1"/>
     <row r="995" ht="14.3" customHeight="1"/>
-    <row r="996" ht="14.3" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2912,8 +2898,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -2965,7 +2951,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.3" customHeight="1">
@@ -2997,7 +2983,7 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">
@@ -3042,10 +3028,10 @@
     </row>
     <row r="12" spans="1:26" ht="14.3" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.3" customHeight="1"/>

</xml_diff>

<commit_message>
update date picker available
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Ptgununghartatransportsolutions/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Portal_Ptgununghartatransportsolutions/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Ptgununghartatransportsolutions\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED222B85-31A6-493C-8DAA-5F53AE393B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F728A578-F095-4E69-943B-1B078F0C3025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -191,6 +191,9 @@
     <t>Captcha_RuleId</t>
   </si>
   <si>
+    <t>[Dev] RPA_Moon_UploadBucket</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -200,6 +203,21 @@
     <t>DialogDownloadChrome</t>
   </si>
   <si>
+    <t>[Dev] RPA_Moon_PathMasterFolder</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_PathMailTemplate</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_PathSaKey</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_PathDownloadChrome</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_DialogDownloadChrome</t>
+  </si>
+  <si>
     <t>SenderName</t>
   </si>
   <si>
@@ -221,37 +239,19 @@
     <t>CaptchaProcess</t>
   </si>
   <si>
+    <t>[Dev] RPA_Moon_PathCaptchaHandler</t>
+  </si>
+  <si>
     <t>PathCaptchaHandler</t>
   </si>
   <si>
+    <t>[Dev] RPA_Moon_SheetIdConfig_Transport</t>
+  </si>
+  <si>
     <t>Traveloka_CaptchaHandler</t>
   </si>
   <si>
     <t>RPA205_GunungHarta_Captcha_SiteKey</t>
-  </si>
-  <si>
-    <t>RPA_Moon_UploadBucket</t>
-  </si>
-  <si>
-    <t>RPA_Moon_SheetIdConfig_Transport</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathMasterFolder</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathMailTemplate</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathSaKey</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathDownloadChrome</t>
-  </si>
-  <si>
-    <t>RPA_Moon_DialogDownloadChrome</t>
-  </si>
-  <si>
-    <t>RPA_Moon_PathCaptchaHandler</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -678,10 +678,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.3" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -719,7 +719,7 @@
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
@@ -727,10 +727,10 @@
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1">
@@ -2898,8 +2898,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -2951,7 +2951,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.3" customHeight="1">
@@ -2959,7 +2959,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.3" customHeight="1">
@@ -2967,7 +2967,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.3" customHeight="1">
@@ -2975,7 +2975,7 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.3" customHeight="1">
@@ -2983,7 +2983,7 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.3" customHeight="1">
@@ -2991,47 +2991,47 @@
         <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.3" customHeight="1">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.3" customHeight="1">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.3" customHeight="1">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.3" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.3" customHeight="1"/>

</xml_diff>